<commit_message>
fix bugs and add block users
</commit_message>
<xml_diff>
--- a/docs/process.xlsx
+++ b/docs/process.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23613"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="100" windowWidth="14800" windowHeight="8020"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8025"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>编号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -62,6 +62,18 @@
   </si>
   <si>
     <t>实现显示好友的最新动态功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>封禁用户</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>郭俊石</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>邀请好友加入小组</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -109,7 +121,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -411,20 +423,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" customWidth="1"/>
-    <col min="5" max="5" width="29.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.625" customWidth="1"/>
+    <col min="4" max="4" width="16.875" customWidth="1"/>
+    <col min="5" max="5" width="29.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,7 +453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -458,7 +470,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -475,7 +487,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -485,11 +497,14 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
+      <c r="D4">
+        <v>11</v>
+      </c>
       <c r="E4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -499,8 +514,45 @@
       <c r="C5" t="s">
         <v>8</v>
       </c>
+      <c r="D5">
+        <v>11</v>
+      </c>
       <c r="E5" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>11.19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>11.19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change access from public to admin of "active posts"
</commit_message>
<xml_diff>
--- a/docs/process.xlsx
+++ b/docs/process.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23613"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14400"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>编号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -94,6 +94,14 @@
   </si>
   <si>
     <t>添加话题管理功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>雷建坤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加管理员查看人气话题的功能</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -460,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -605,7 +613,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="2">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
         <v>15</v>
@@ -622,7 +630,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="2">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
         <v>16</v>
@@ -639,10 +647,27 @@
         <v>17</v>
       </c>
       <c r="D10" s="2">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>41598</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="2">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add delete confirm dialog
</commit_message>
<xml_diff>
--- a/docs/process.xlsx
+++ b/docs/process.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23613"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14445"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>编号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -118,6 +118,14 @@
   </si>
   <si>
     <t>审核系统的构建</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>雷建坤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加内容访问次数统计的功能</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -182,7 +190,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -484,22 +492,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="2"/>
-    <col min="2" max="2" width="11.125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="29.875" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="11.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="29.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -516,7 +524,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -533,7 +541,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -550,7 +558,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -567,7 +575,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -584,7 +592,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -601,7 +609,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -618,7 +626,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -635,7 +643,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -652,7 +660,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -669,7 +677,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -686,7 +694,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -703,7 +711,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -715,6 +723,20 @@
       </c>
       <c r="E13" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>41599</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>